<commit_message>
ajuste de endpoints para que funcionen en el frontend
</commit_message>
<xml_diff>
--- a/src/routes/calendarioTest.xlsx
+++ b/src/routes/calendarioTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgfch\Desktop\calendarP\src\routes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34531B4-D8BD-485B-8CCB-4565930C5B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D437E7C3-CCB4-493D-858C-EBB7FD41012E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="23426" windowHeight="14980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Materia</t>
   </si>
@@ -92,6 +92,36 @@
   </si>
   <si>
     <t>JUEVES 06:00-08:00 SA414</t>
+  </si>
+  <si>
+    <t>1155105A</t>
+  </si>
+  <si>
+    <t>INTRODUCCION ING SISTEMAS</t>
+  </si>
+  <si>
+    <t>MARTES 08:00-09:00 SF404</t>
+  </si>
+  <si>
+    <t>JUEVES 08:00-10:00 SA403</t>
+  </si>
+  <si>
+    <t>1155201A</t>
+  </si>
+  <si>
+    <t>MARTES 06:00-08:00 SA203</t>
+  </si>
+  <si>
+    <t>JUEVES 06:00-08:00 SA202</t>
+  </si>
+  <si>
+    <t>1155102A</t>
+  </si>
+  <si>
+    <t>MARTES 10:00-12:00 SA402</t>
+  </si>
+  <si>
+    <t>MIERCOLES 09:00-10:00 SA414</t>
   </si>
 </sst>
 </file>
@@ -616,10 +646,28 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -988,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1018,13 +1066,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="10">
         <v>6079</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1032,21 +1080,21 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="10">
         <v>7491</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1054,21 +1102,21 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="10">
         <v>5159</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1076,21 +1124,21 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="10">
         <v>1496</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1098,21 +1146,21 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="10">
         <v>1713</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1120,15 +1168,87 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1827</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="10">
+        <v>7491</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10">
+        <v>4412</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="24">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1144,7 +1264,11 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>